<commit_message>
Week 14: Release 0.3
</commit_message>
<xml_diff>
--- a/y2s1/statistics-ii/tutorials/stat2t9.xlsx
+++ b/y2s1/statistics-ii/tutorials/stat2t9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user300\repo\dco-1820\y2s1\statistics-ii\tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706741D4-CED2-430D-B069-979C5FDD458C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B4FFB3-6265-40BE-852B-BF1D4E383D16}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="580" windowWidth="14400" windowHeight="7440" activeTab="5" xr2:uid="{DBB35EE7-C701-497C-9608-BD395BF20AB9}"/>
+    <workbookView xWindow="2060" yWindow="730" windowWidth="14400" windowHeight="7440" activeTab="8" xr2:uid="{DBB35EE7-C701-497C-9608-BD395BF20AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="T9Q1" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,10 @@
     <sheet name="T9Q3" sheetId="5" r:id="rId3"/>
     <sheet name="T9Q4" sheetId="6" r:id="rId4"/>
     <sheet name="T9Q5" sheetId="7" r:id="rId5"/>
-    <sheet name="T9Q6-END" sheetId="2" r:id="rId6"/>
+    <sheet name="Q6" sheetId="8" r:id="rId6"/>
+    <sheet name="Q7" sheetId="9" r:id="rId7"/>
+    <sheet name="Q8" sheetId="10" r:id="rId8"/>
+    <sheet name="Q9" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="116">
   <si>
     <t>Average Price</t>
   </si>
@@ -59,9 +62,6 @@
     <t>SUM</t>
   </si>
   <si>
-    <t>Answer:</t>
-  </si>
-  <si>
     <t>WQ0</t>
   </si>
   <si>
@@ -98,39 +98,15 @@
     <t>Quantity in 2010</t>
   </si>
   <si>
-    <t>q0p0</t>
-  </si>
-  <si>
-    <t>q0p1</t>
-  </si>
-  <si>
-    <t>q1p0</t>
-  </si>
-  <si>
-    <t>q1p1</t>
-  </si>
-  <si>
     <t>LQI</t>
   </si>
   <si>
     <t>PQI</t>
   </si>
   <si>
-    <t>p0q0</t>
-  </si>
-  <si>
-    <t>p1q1</t>
-  </si>
-  <si>
-    <t>Q6. The following table lists the quantities and costs of materials of a company for two years.</t>
-  </si>
-  <si>
     <t>Quantity ( tonnes )</t>
   </si>
   <si>
-    <t>Cost ( RM’000 )</t>
-  </si>
-  <si>
     <t>Material</t>
   </si>
   <si>
@@ -140,72 +116,9 @@
     <t>Year2</t>
   </si>
   <si>
-    <t>Using the year 1 as the base year, calculate the</t>
-  </si>
-  <si>
-    <t>(a) price ( cost ) relative index for material A in year 2,</t>
-  </si>
-  <si>
-    <t>(b) quantity relative index for material C in year 2,</t>
-  </si>
-  <si>
-    <t>(c) simple aggregate price and quantity indices for year 2,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simple aggregate price indices: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simple aggregate quantity indices: </t>
-  </si>
-  <si>
-    <t>(d) simple average of price and quantity relative indices for year 2,</t>
-  </si>
-  <si>
     <t>p1/p0*100</t>
   </si>
   <si>
-    <t>q1/q0*100</t>
-  </si>
-  <si>
-    <t>simple average of price index</t>
-  </si>
-  <si>
-    <t>simple average of quantity relative index</t>
-  </si>
-  <si>
-    <t>(e) Laspeyres, Paasche and Fisher’s Ideal price indices for year 2,</t>
-  </si>
-  <si>
-    <t>LPI:</t>
-  </si>
-  <si>
-    <t>PPI:</t>
-  </si>
-  <si>
-    <t>FIPI:</t>
-  </si>
-  <si>
-    <t>Laspeyres, Paasche and Fisher’s Ideal quantity indices for year 2,</t>
-  </si>
-  <si>
-    <t>p0q1</t>
-  </si>
-  <si>
-    <t>p1q0</t>
-  </si>
-  <si>
-    <t>FIQI</t>
-  </si>
-  <si>
-    <t>(g) value index for year 2.</t>
-  </si>
-  <si>
-    <t>VAL INDEX</t>
-  </si>
-  <si>
-    <t>Q7. The profits of two companies, A and B, expressed in terms of index numbers are given below.</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -221,24 +134,6 @@
     <t>CompanyBAdjusted</t>
   </si>
   <si>
-    <t>After changing base, we can see that the growth of profits s faster in company B than company A</t>
-  </si>
-  <si>
-    <t>Q8. In January 2009, a factory paid out a total of RM 64,000 to 120 employees on the payroll.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In July 2009, the factory had 30 more employees on the payroll and paid out RM 11,800 more than in January 2009. Using January 2009 as the base month, calculate the</t>
-  </si>
-  <si>
-    <t>(a) labour expenses index number ( value relative ) for July 2009,</t>
-  </si>
-  <si>
-    <t>(b) employee index number ( quantity relative ) for July 2009.</t>
-  </si>
-  <si>
-    <t>Q9</t>
-  </si>
-  <si>
     <t>Expenditure on petrol and servicing ( $’000 )</t>
   </si>
   <si>
@@ -402,13 +297,103 @@
   </si>
   <si>
     <t>h)</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost ( RM’000 ) </t>
+  </si>
+  <si>
+    <t>Qty.Rel.Ind</t>
+  </si>
+  <si>
+    <t>Cos.Rel.In</t>
+  </si>
+  <si>
+    <t>Q0P0</t>
+  </si>
+  <si>
+    <t>Q0P1</t>
+  </si>
+  <si>
+    <t>Q1P0</t>
+  </si>
+  <si>
+    <t>Q1P1</t>
+  </si>
+  <si>
+    <t>Aggr.Price</t>
+  </si>
+  <si>
+    <t>Aggr.Qty</t>
+  </si>
+  <si>
+    <t>Avg.Price</t>
+  </si>
+  <si>
+    <t>Avg.Qty</t>
+  </si>
+  <si>
+    <t>LPI</t>
+  </si>
+  <si>
+    <t>PPI</t>
+  </si>
+  <si>
+    <t>FIP</t>
+  </si>
+  <si>
+    <t>FIQ</t>
+  </si>
+  <si>
+    <t>Val.Index</t>
+  </si>
+  <si>
+    <t>Question 7</t>
+  </si>
+  <si>
+    <t>Comment:</t>
+  </si>
+  <si>
+    <t>The growth of profits in company A is faster than company B</t>
+  </si>
+  <si>
+    <t>Question 8</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Employeees</t>
+  </si>
+  <si>
+    <t>P.Rel</t>
+  </si>
+  <si>
+    <t>V.Rel</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>Val.Rel</t>
+  </si>
+  <si>
+    <t>Qty.Rel.</t>
+  </si>
+  <si>
+    <t>Question 9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,14 +403,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -516,15 +493,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -534,8 +509,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,30 +836,30 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -911,10 +887,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -949,12 +925,12 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="C7">
         <f>C3/B3*100</f>
@@ -999,38 +975,38 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="I2" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -1060,7 +1036,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -1090,7 +1066,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1120,7 +1096,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -1183,7 +1159,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="B9">
         <f>E5/D5*100</f>
@@ -1192,7 +1168,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="B10">
         <f>E7/D7*100</f>
@@ -1201,7 +1177,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <f>1/4*SUM(F3:F6)</f>
@@ -1210,7 +1186,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <f>1/C7*G7</f>
@@ -1219,7 +1195,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B13">
         <f>I7/H7*100</f>
@@ -1251,12 +1227,12 @@
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1372,11 +1348,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
+      <c r="A8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <f>E3/C3*100</f>
@@ -1385,7 +1361,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B10">
         <f>D7/C7*100</f>
@@ -1394,10 +1370,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="D11" s="2">
         <v>2007</v>
@@ -1409,16 +1385,16 @@
         <v>2010</v>
       </c>
       <c r="G11" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="I11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" t="s">
         <v>8</v>
-      </c>
-      <c r="J11" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1568,7 +1544,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <f>1/4*G16</f>
@@ -1577,7 +1553,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="B19">
         <f>1/C16*H16</f>
@@ -1586,7 +1562,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B20">
         <f>J16/I16*100</f>
@@ -1617,30 +1593,30 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B3">
         <v>103.4</v>
@@ -1663,7 +1639,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -1690,7 +1666,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B5">
         <f>B3*B4</f>
@@ -1723,7 +1699,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="C7">
         <f>H5/H4</f>
@@ -1748,43 +1724,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
       <c r="G1" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="H1" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="J1" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="L1" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="M1" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -1879,7 +1855,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="C4">
         <f>SUM(C2:C3)</f>
@@ -1928,7 +1904,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <f>G2</f>
@@ -1937,7 +1913,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="B6">
         <f>H3</f>
@@ -1946,7 +1922,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <f>I2</f>
@@ -1955,7 +1931,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="B8">
         <f>L4/J4*100</f>
@@ -1964,7 +1940,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B9">
         <f>M4/K4*100</f>
@@ -1973,7 +1949,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="B10">
         <f>K4/J4*100</f>
@@ -1982,7 +1958,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="B11">
         <f>M4/L4*100</f>
@@ -1991,7 +1967,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="B12">
         <f>M4/J4*100</f>
@@ -2005,956 +1981,737 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A2C1F8-0B34-4C17-A63D-E49808DFA213}">
-  <dimension ref="A1:I87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D6D74B-FD16-42F8-98B5-D412F1BC1442}">
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C3" s="9"/>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>175</v>
+      </c>
+      <c r="E4">
+        <v>201</v>
+      </c>
+      <c r="F4">
+        <v>15.4</v>
+      </c>
+      <c r="G4">
+        <v>18.3</v>
+      </c>
+      <c r="H4">
+        <f>E4/D4*100</f>
+        <v>114.85714285714286</v>
+      </c>
+      <c r="I4">
+        <f>G4/F4*100</f>
+        <v>118.83116883116884</v>
+      </c>
+      <c r="J4">
+        <f>D4*F4</f>
+        <v>2695</v>
+      </c>
+      <c r="K4">
+        <f>D4*G4</f>
+        <v>3202.5</v>
+      </c>
+      <c r="L4">
+        <f>E4*F4</f>
+        <v>3095.4</v>
+      </c>
+      <c r="M4">
+        <f>E4*G4</f>
+        <v>3678.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>175</v>
-      </c>
-      <c r="C4">
-        <v>201</v>
-      </c>
-      <c r="D4">
-        <v>15.4</v>
-      </c>
-      <c r="E4">
-        <v>18.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>32</v>
-      </c>
-      <c r="C5">
+      <c r="E5">
         <v>46</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>12.7</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>14.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="H5">
+        <f t="shared" ref="H5:H6" si="0">E5/D5*100</f>
+        <v>143.75</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I6" si="1">G5/F5*100</f>
+        <v>117.3228346456693</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J6" si="2">D5*F5</f>
+        <v>406.4</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K6" si="3">D5*G5</f>
+        <v>476.8</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L6" si="4">E5*F5</f>
+        <v>584.19999999999993</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M6" si="5">E5*G5</f>
+        <v>685.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="D6">
         <v>48</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>43</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>27.6</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>89.583333333333343</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>90.217391304347814</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>1324.8000000000002</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>1195.1999999999998</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>1186.8</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>1070.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7">
+        <f>SUM(D4:D6)</f>
+        <v>255</v>
+      </c>
+      <c r="E7">
+        <f>SUM(E4:E6)</f>
+        <v>290</v>
+      </c>
+      <c r="F7">
+        <f>SUM(F4:F6)</f>
+        <v>55.7</v>
+      </c>
+      <c r="G7">
+        <f>SUM(G4:G6)</f>
+        <v>58.1</v>
+      </c>
+      <c r="H7">
+        <f>SUM(H4:H6)</f>
+        <v>348.19047619047626</v>
+      </c>
+      <c r="I7">
+        <f>SUM(I4:I6)</f>
+        <v>326.37139478118593</v>
+      </c>
+      <c r="J7">
+        <f>SUM(J4:J6)</f>
+        <v>4426.2000000000007</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:M7" si="6">SUM(K4:K6)</f>
+        <v>4874.5</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="6"/>
+        <v>4866.3999999999996</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="6"/>
+        <v>5434.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="B9">
+        <f>G4/F4*100</f>
+        <v>118.83116883116884</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10">
+        <f>E6/D6*100</f>
+        <v>89.583333333333343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <f>E4/D4*100</f>
-        <v>118.83116883116884</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11">
+        <f>G7/F7*100</f>
+        <v>104.30879712746859</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12">
+        <f>E7/D7*100</f>
+        <v>113.72549019607843</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13">
+        <f>I7/3</f>
+        <v>108.79046492706198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14">
+        <f>H7/3</f>
+        <v>116.06349206349209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15">
-        <f>C6/B6*100</f>
-        <v>89.583333333333343</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19">
-        <f>SUM(E4:E6)/SUM(D4:D6)*100</f>
-        <v>104.30879712746859</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20">
-        <f>SUM(C4:C6)/SUM(B4:B6)*100</f>
-        <v>113.72549019607843</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26">
-        <v>175</v>
-      </c>
-      <c r="C26">
-        <v>201</v>
-      </c>
-      <c r="D26">
-        <v>15.4</v>
-      </c>
-      <c r="E26">
-        <v>18.3</v>
-      </c>
-      <c r="F26">
-        <f>E26/D26*100</f>
-        <v>118.83116883116884</v>
-      </c>
-      <c r="G26">
-        <f>C26/B26*100</f>
-        <v>114.85714285714286</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27">
-        <v>32</v>
-      </c>
-      <c r="C27">
-        <v>46</v>
-      </c>
-      <c r="D27">
-        <v>12.7</v>
-      </c>
-      <c r="E27">
-        <v>14.9</v>
-      </c>
-      <c r="F27">
-        <f t="shared" ref="F27:F28" si="0">E27/D27*100</f>
-        <v>117.3228346456693</v>
-      </c>
-      <c r="G27">
-        <f t="shared" ref="G27:G28" si="1">C27/B27*100</f>
-        <v>143.75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28">
-        <v>48</v>
-      </c>
-      <c r="C28">
-        <v>43</v>
-      </c>
-      <c r="D28">
-        <v>27.6</v>
-      </c>
-      <c r="E28">
-        <v>24.9</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="0"/>
-        <v>90.217391304347814</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="1"/>
-        <v>89.583333333333343</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30">
-        <f>SUM(F26:F28)/COUNT(F26:F28)</f>
-        <v>108.79046492706198</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31">
-        <f>SUM(G26:G28)/COUNT(G26:G28)</f>
-        <v>116.06349206349209</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B35" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" t="s">
-        <v>32</v>
-      </c>
-      <c r="E36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15">
+        <f>K7/J7*100</f>
+        <v>110.12832678143778</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16">
+        <f>M7/L7*100</f>
+        <v>111.6718724313661</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17">
+        <f>SQRT(C15*C16)</f>
+        <v>110.89741412411976</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <f>L7/J7*100</f>
+        <v>109.94532556142964</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="G36" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37">
-        <v>175</v>
-      </c>
-      <c r="C37">
-        <v>201</v>
-      </c>
-      <c r="D37">
-        <v>15.4</v>
-      </c>
-      <c r="E37">
-        <v>18.3</v>
-      </c>
-      <c r="F37">
-        <f>B37*D37</f>
-        <v>2695</v>
-      </c>
-      <c r="G37">
-        <f>B37*E37</f>
-        <v>3202.5</v>
-      </c>
-      <c r="H37">
-        <f>C37*D37</f>
-        <v>3095.4</v>
-      </c>
-      <c r="I37">
-        <f>C37*E37</f>
-        <v>3678.3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38">
-        <v>32</v>
-      </c>
-      <c r="C38">
-        <v>46</v>
-      </c>
-      <c r="D38">
-        <v>12.7</v>
-      </c>
-      <c r="E38">
-        <v>14.9</v>
-      </c>
-      <c r="F38">
-        <f>B38*D38</f>
-        <v>406.4</v>
-      </c>
-      <c r="G38">
-        <f t="shared" ref="G38:G39" si="2">B38*E38</f>
-        <v>476.8</v>
-      </c>
-      <c r="H38">
-        <f t="shared" ref="H38:H39" si="3">C38*D38</f>
-        <v>584.19999999999993</v>
-      </c>
-      <c r="I38">
-        <f t="shared" ref="I38:I39" si="4">C38*E38</f>
-        <v>685.4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39">
-        <v>48</v>
-      </c>
-      <c r="C39">
-        <v>43</v>
-      </c>
-      <c r="D39">
-        <v>27.6</v>
-      </c>
-      <c r="E39">
-        <v>24.9</v>
-      </c>
-      <c r="F39" s="5">
-        <f>B39*D39</f>
-        <v>1324.8000000000002</v>
-      </c>
-      <c r="G39" s="5">
-        <f t="shared" si="2"/>
-        <v>1195.1999999999998</v>
-      </c>
-      <c r="H39" s="5">
-        <f t="shared" si="3"/>
-        <v>1186.8</v>
-      </c>
-      <c r="I39" s="5">
-        <f t="shared" si="4"/>
-        <v>1070.7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F40" s="5">
-        <f>SUM(F37:F39)</f>
-        <v>4426.2000000000007</v>
-      </c>
-      <c r="G40" s="5">
-        <f>SUM(G37:G39)</f>
-        <v>4874.5</v>
-      </c>
-      <c r="H40" s="5">
-        <f>SUM(H37:H39)</f>
-        <v>4866.3999999999996</v>
-      </c>
-      <c r="I40" s="5">
-        <f>SUM(I37:I39)</f>
-        <v>5434.4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41">
-        <f>G40/F40*100</f>
-        <v>110.12832678143778</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42">
-        <f>I40/H40*100</f>
-        <v>111.6718724313661</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43">
-        <f>SQRT(B41*B42)</f>
-        <v>110.89741412411976</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B47" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>31</v>
-      </c>
-      <c r="B48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" t="s">
-        <v>32</v>
-      </c>
-      <c r="E48" t="s">
-        <v>33</v>
-      </c>
-      <c r="F48" t="s">
-        <v>26</v>
-      </c>
-      <c r="G48" t="s">
-        <v>50</v>
-      </c>
-      <c r="H48" t="s">
-        <v>51</v>
-      </c>
-      <c r="I48" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49">
-        <v>175</v>
-      </c>
-      <c r="C49">
-        <v>201</v>
-      </c>
-      <c r="D49">
-        <v>15.4</v>
-      </c>
-      <c r="E49">
-        <v>18.3</v>
-      </c>
-      <c r="F49">
-        <f>B49*D49</f>
-        <v>2695</v>
-      </c>
-      <c r="G49">
-        <f>C49*D49</f>
-        <v>3095.4</v>
-      </c>
-      <c r="H49">
-        <f>B49*E49</f>
-        <v>3202.5</v>
-      </c>
-      <c r="I49">
-        <f>C49*E49</f>
-        <v>3678.3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50">
-        <v>32</v>
-      </c>
-      <c r="C50">
-        <v>46</v>
-      </c>
-      <c r="D50">
-        <v>12.7</v>
-      </c>
-      <c r="E50">
-        <v>14.9</v>
-      </c>
-      <c r="F50">
-        <f>B50*D50</f>
-        <v>406.4</v>
-      </c>
-      <c r="G50">
-        <f t="shared" ref="G50:G51" si="5">C50*D50</f>
-        <v>584.19999999999993</v>
-      </c>
-      <c r="H50">
-        <f t="shared" ref="H50:H51" si="6">B50*E50</f>
-        <v>476.8</v>
-      </c>
-      <c r="I50">
-        <f t="shared" ref="I50:I51" si="7">C50*E50</f>
-        <v>685.4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51">
-        <v>48</v>
-      </c>
-      <c r="C51">
-        <v>43</v>
-      </c>
-      <c r="D51">
-        <v>27.6</v>
-      </c>
-      <c r="E51">
-        <v>24.9</v>
-      </c>
-      <c r="F51" s="5">
-        <f>B51*D51</f>
-        <v>1324.8000000000002</v>
-      </c>
-      <c r="G51">
-        <f t="shared" si="5"/>
-        <v>1186.8</v>
-      </c>
-      <c r="H51">
-        <f t="shared" si="6"/>
-        <v>1195.1999999999998</v>
-      </c>
-      <c r="I51" s="5">
-        <f t="shared" si="7"/>
-        <v>1070.7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F52" s="5">
-        <f>SUM(F49:F51)</f>
-        <v>4426.2000000000007</v>
-      </c>
-      <c r="G52" s="5">
-        <f>SUM(G49:G51)</f>
-        <v>4866.3999999999996</v>
-      </c>
-      <c r="H52" s="5">
-        <f>SUM(H49:H51)</f>
-        <v>4874.5</v>
-      </c>
-      <c r="I52" s="5">
-        <f>SUM(I49:I51)</f>
-        <v>5434.4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>24</v>
-      </c>
-      <c r="B54">
-        <f>G52/F52*100</f>
-        <v>109.94532556142964</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55">
-        <f>I52/H52*100</f>
+      <c r="C19">
+        <f>M7/K7*100</f>
         <v>111.48630628782439</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56">
-        <f>SQRT(B54*B55)</f>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20">
+        <f>SQRT(C18*C19)</f>
         <v>110.71313490483463</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>54</v>
-      </c>
-      <c r="B60">
-        <f>I52/F52*100</f>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21">
+        <f>M7/J7*100</f>
         <v>122.77800370520985</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>56</v>
-      </c>
-      <c r="B64">
-        <v>2004</v>
-      </c>
-      <c r="C64">
-        <v>2005</v>
-      </c>
-      <c r="D64">
-        <v>2006</v>
-      </c>
-      <c r="E64">
-        <v>2007</v>
-      </c>
-      <c r="F64">
-        <v>2008</v>
-      </c>
-      <c r="G64">
-        <v>2009</v>
-      </c>
-      <c r="H64">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>57</v>
-      </c>
-      <c r="B65" t="s">
-        <v>58</v>
-      </c>
-      <c r="C65" t="s">
-        <v>58</v>
-      </c>
-      <c r="D65">
-        <v>100</v>
-      </c>
-      <c r="E65">
-        <v>110.61</v>
-      </c>
-      <c r="F65">
-        <v>123.45</v>
-      </c>
-      <c r="G65">
-        <v>136.22999999999999</v>
-      </c>
-      <c r="H65">
-        <v>151.16</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>59</v>
-      </c>
-      <c r="B66">
-        <v>100</v>
-      </c>
-      <c r="C66">
-        <v>109.16</v>
-      </c>
-      <c r="D66">
-        <v>118.32</v>
-      </c>
-      <c r="E66">
-        <v>127.61</v>
-      </c>
-      <c r="F66">
-        <v>136.21</v>
-      </c>
-      <c r="G66">
-        <v>145.56</v>
-      </c>
-      <c r="H66">
-        <v>156.22999999999999</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B67">
-        <f>B66/D66*100</f>
-        <v>84.516565246788375</v>
-      </c>
-      <c r="C67">
-        <f>C66/D66*100</f>
-        <v>92.25828262339418</v>
-      </c>
-      <c r="D67">
-        <f>D66/D66*100</f>
-        <v>100</v>
-      </c>
-      <c r="E67">
-        <f>E66/D66*100</f>
-        <v>107.85158891142666</v>
-      </c>
-      <c r="F67">
-        <f>F66/E66*100</f>
-        <v>106.73928375519162</v>
-      </c>
-      <c r="G67">
-        <f>G66/D66*100</f>
-        <v>123.02231237322516</v>
-      </c>
-      <c r="H67">
-        <f>H66/D66*100</f>
-        <v>132.04022988505747</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <f>(64000+11800)/(64000)*100</f>
-        <v>118.4375</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A80">
-        <f>150/120*100</f>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>56</v>
-      </c>
-      <c r="B84">
-        <v>2004</v>
-      </c>
-      <c r="C84">
-        <v>2005</v>
-      </c>
-      <c r="D84">
-        <v>2006</v>
-      </c>
-      <c r="E84">
-        <v>2007</v>
-      </c>
-      <c r="F84">
-        <v>2008</v>
-      </c>
-      <c r="G84">
-        <v>2009</v>
-      </c>
-      <c r="H84">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>67</v>
-      </c>
-      <c r="B85">
-        <v>166</v>
-      </c>
-      <c r="C85">
-        <v>220</v>
-      </c>
-      <c r="D85">
-        <v>360</v>
-      </c>
-      <c r="E85">
-        <v>528</v>
-      </c>
-      <c r="F85">
-        <v>664</v>
-      </c>
-      <c r="G85">
-        <v>763</v>
-      </c>
-      <c r="H85">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>68</v>
-      </c>
-      <c r="B86">
-        <v>111</v>
-      </c>
-      <c r="C86">
-        <v>147</v>
-      </c>
-      <c r="D86">
-        <v>182</v>
-      </c>
-      <c r="E86">
-        <v>211</v>
-      </c>
-      <c r="F86">
-        <v>228</v>
-      </c>
-      <c r="G86">
-        <v>251</v>
-      </c>
-      <c r="H86">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>69</v>
-      </c>
-      <c r="B87">
-        <f>B85/B86*100</f>
-        <v>149.54954954954957</v>
-      </c>
-      <c r="C87">
-        <f t="shared" ref="C87:H87" si="8">C85/C86*100</f>
-        <v>149.65986394557825</v>
-      </c>
-      <c r="D87">
-        <f t="shared" si="8"/>
-        <v>197.80219780219781</v>
-      </c>
-      <c r="E87">
-        <f t="shared" si="8"/>
-        <v>250.23696682464455</v>
-      </c>
-      <c r="F87">
-        <f t="shared" si="8"/>
-        <v>291.22807017543863</v>
-      </c>
-      <c r="G87">
-        <f t="shared" si="8"/>
-        <v>303.98406374501991</v>
-      </c>
-      <c r="H87">
-        <f t="shared" si="8"/>
-        <v>350.76923076923077</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B2:C2"/>
+  <mergeCells count="3">
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0D8C4B-03A2-4DAE-A042-CCB39F0E4102}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>2004</v>
+      </c>
+      <c r="D3">
+        <v>2005</v>
+      </c>
+      <c r="E3">
+        <v>2006</v>
+      </c>
+      <c r="F3">
+        <v>2007</v>
+      </c>
+      <c r="G3">
+        <v>2008</v>
+      </c>
+      <c r="H3">
+        <v>2009</v>
+      </c>
+      <c r="I3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>110.61</v>
+      </c>
+      <c r="G4">
+        <v>123.45</v>
+      </c>
+      <c r="H4">
+        <v>136.22999999999999</v>
+      </c>
+      <c r="I4">
+        <v>151.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>109.16</v>
+      </c>
+      <c r="E5">
+        <v>118.32</v>
+      </c>
+      <c r="F5">
+        <v>127.61</v>
+      </c>
+      <c r="G5">
+        <v>136.21</v>
+      </c>
+      <c r="H5">
+        <v>145.56</v>
+      </c>
+      <c r="I5">
+        <v>156.22999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <f>C5/118.32*100</f>
+        <v>84.516565246788375</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:I6" si="0">D5/118.32*100</f>
+        <v>92.25828262339418</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>107.85158891142666</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>115.12001352265044</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>123.02231237322516</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>132.04022988505747</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B725ABA6-305A-4539-A0A1-50A36320655F}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4">
+        <v>64000</v>
+      </c>
+      <c r="D4">
+        <v>120</v>
+      </c>
+      <c r="F4">
+        <f>C5/C4*100</f>
+        <v>118.4375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5">
+        <f>C4+11800</f>
+        <v>75800</v>
+      </c>
+      <c r="D5">
+        <f>D4+30</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7">
+        <f>C5/C4*100</f>
+        <v>118.4375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8">
+        <f>D5/D4*100</f>
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4104439-5D3D-4B79-BE61-2E8B8E3529E6}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>2004</v>
+      </c>
+      <c r="D3">
+        <v>2005</v>
+      </c>
+      <c r="E3">
+        <v>2006</v>
+      </c>
+      <c r="F3">
+        <v>2007</v>
+      </c>
+      <c r="G3">
+        <v>2008</v>
+      </c>
+      <c r="H3">
+        <v>2009</v>
+      </c>
+      <c r="I3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>166</v>
+      </c>
+      <c r="D4">
+        <v>220</v>
+      </c>
+      <c r="E4">
+        <v>360</v>
+      </c>
+      <c r="F4">
+        <v>528</v>
+      </c>
+      <c r="G4">
+        <v>664</v>
+      </c>
+      <c r="H4">
+        <v>763</v>
+      </c>
+      <c r="I4">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>111</v>
+      </c>
+      <c r="D5">
+        <v>147</v>
+      </c>
+      <c r="E5">
+        <v>182</v>
+      </c>
+      <c r="F5">
+        <v>211</v>
+      </c>
+      <c r="G5">
+        <v>228</v>
+      </c>
+      <c r="H5">
+        <v>251</v>
+      </c>
+      <c r="I5">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <f>C4*100/C5</f>
+        <v>149.54954954954954</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:I6" si="0">D4*100/D5</f>
+        <v>149.65986394557822</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>197.80219780219781</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>250.23696682464455</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>291.22807017543857</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>303.98406374501991</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>350.76923076923077</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>